<commit_message>
Edit index page for import books
</commit_message>
<xml_diff>
--- a/BookStoreAdminApplication/BookStoreAdminApplication/files/Books.xlsx
+++ b/BookStoreAdminApplication/BookStoreAdminApplication/files/Books.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Desktop\IS-project\BookStoreAdminApplication\BookStoreAdminApplication\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Desktop\IS-project\BookStore\BookStoreAdminApplication\BookStoreAdminApplication\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3FEA7B-6CCE-4DB4-A413-C227B711BB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF0AD8D-4A62-42E3-A201-BFD243B39088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3ECC8FCD-9CF5-408B-9D8B-5CDB973ADA74}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>[3,5]</t>
   </si>
   <si>
-    <t>Memory4</t>
+    <t>Memory2</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
         <v>2022</v>
       </c>
       <c r="D2">
-        <v>178367342</v>
+        <v>178367343</v>
       </c>
       <c r="E2" s="2">
         <v>350</v>

</xml_diff>